<commit_message>
Solucionar errores, menu y arbol realizado
</commit_message>
<xml_diff>
--- a/proyecto final/Prueba2.xlsx
+++ b/proyecto final/Prueba2.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>CC</t>
+          <t>Cédula</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -450,52 +450,59 @@
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Diagnóstico</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Síntomas</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1212</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>nan</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>nan</t>
-        </is>
+          <t>jose</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>18</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Cáncer de Pulmón</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>[1, 1, 1, 1, 1]</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1107978061</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2222</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>jose</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+          <t>juan</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>18</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>tos</t>
+          <t>Cáncer de Pulmón</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>[0, 0, 0, 0, 0]</t>
         </is>
       </c>
     </row>

</xml_diff>